<commit_message>
CRUD ready to use, létrehoztam teszt adatokat sql
</commit_message>
<xml_diff>
--- a/document_database/Adatgyűjtés/országok történetei.xlsx
+++ b/document_database/Adatgyűjtés/országok történetei.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84ECB854-38ED-4EAC-B961-231EE4EFBC49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C0E3429-A07C-4E89-8FE1-409D0B2B840C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="85">
   <si>
     <t>Magyarország</t>
   </si>
@@ -272,6 +272,9 @@
   </si>
   <si>
     <t>Németország</t>
+  </si>
+  <si>
+    <t>500-751</t>
   </si>
 </sst>
 </file>
@@ -709,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:AI70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I70" sqref="I70"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M70" sqref="M70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1403,6 +1406,10 @@
       </c>
       <c r="G70" s="16"/>
       <c r="H70" s="16"/>
+      <c r="I70" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="M70" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Német történelem haladás (még sok hátravan)
</commit_message>
<xml_diff>
--- a/document_database/Adatgyűjtés/országok történetei.xlsx
+++ b/document_database/Adatgyűjtés/országok történetei.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C0E3429-A07C-4E89-8FE1-409D0B2B840C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47303C6-1693-4BBB-BA7F-C0ADD7096C38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="128">
   <si>
     <t>Magyarország</t>
   </si>
@@ -275,6 +275,135 @@
   </si>
   <si>
     <t>500-751</t>
+  </si>
+  <si>
+    <t>Merovingok</t>
+  </si>
+  <si>
+    <t>https://hu.wikipedia.org/wiki/N%C3%A9metorsz%C3%A1g_t%C3%B6rt%C3%A9nelme</t>
+  </si>
+  <si>
+    <t>751-911</t>
+  </si>
+  <si>
+    <t>Karolingok</t>
+  </si>
+  <si>
+    <t>Merovingok.txt</t>
+  </si>
+  <si>
+    <t>919-1024</t>
+  </si>
+  <si>
+    <t>Az Ottók uralma</t>
+  </si>
+  <si>
+    <t>Karolingok.txt</t>
+  </si>
+  <si>
+    <t>Ottók.txt</t>
+  </si>
+  <si>
+    <t>1024-1125</t>
+  </si>
+  <si>
+    <t>A Száli-ház</t>
+  </si>
+  <si>
+    <t>1138-1254</t>
+  </si>
+  <si>
+    <t>A Stauf-ház</t>
+  </si>
+  <si>
+    <t>Stauf-ház.txt</t>
+  </si>
+  <si>
+    <t>Száli-ház.txt</t>
+  </si>
+  <si>
+    <t>1254-1313</t>
+  </si>
+  <si>
+    <t>Interregnum és a Habsburgok felemelkedése</t>
+  </si>
+  <si>
+    <t>Interregnum és Habsburgok.txt</t>
+  </si>
+  <si>
+    <t>1378-1493</t>
+  </si>
+  <si>
+    <t>A Habsburg-korszak kezdete</t>
+  </si>
+  <si>
+    <t>Habsburg.txt</t>
+  </si>
+  <si>
+    <t>1486-1519</t>
+  </si>
+  <si>
+    <t>I. Miksa uralkodása</t>
+  </si>
+  <si>
+    <t>Miksa.txt</t>
+  </si>
+  <si>
+    <t>Reformáció</t>
+  </si>
+  <si>
+    <t>Reformáció.txt</t>
+  </si>
+  <si>
+    <t>1618-1648</t>
+  </si>
+  <si>
+    <t>A harmincéves háború</t>
+  </si>
+  <si>
+    <t>Harmincéves háború.txt</t>
+  </si>
+  <si>
+    <t>1799-1815</t>
+  </si>
+  <si>
+    <t>Napóleoni háborúk</t>
+  </si>
+  <si>
+    <t>Napóleon.txt</t>
+  </si>
+  <si>
+    <t>1815-1848</t>
+  </si>
+  <si>
+    <t>Német szövetség és a Szent Szövetség</t>
+  </si>
+  <si>
+    <t>Szövetségek.txt</t>
+  </si>
+  <si>
+    <t>48-as német forradalom Berlinben</t>
+  </si>
+  <si>
+    <t>Német 48-as forradalom</t>
+  </si>
+  <si>
+    <t>porosz-osztrák háború</t>
+  </si>
+  <si>
+    <t>porosz-osztrák.txt</t>
+  </si>
+  <si>
+    <t>Német Császárság megalakulása</t>
+  </si>
+  <si>
+    <t>Három császár éve</t>
+  </si>
+  <si>
+    <t>Német Császárság.txt</t>
+  </si>
+  <si>
+    <t>Három császár éve.txt</t>
   </si>
 </sst>
 </file>
@@ -710,10 +839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:AI70"/>
+  <dimension ref="B3:AI100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M70" sqref="M70"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X101" sqref="X101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1367,7 +1496,7 @@
       <c r="G64" s="11"/>
       <c r="H64" s="15"/>
     </row>
-    <row r="65" spans="6:24" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="65" spans="6:33" ht="26.25" x14ac:dyDescent="0.4">
       <c r="F65" s="11"/>
       <c r="G65" s="11"/>
       <c r="H65" s="15"/>
@@ -1381,12 +1510,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="66" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="66" spans="6:33" x14ac:dyDescent="0.25">
       <c r="F66" s="11"/>
       <c r="G66" s="11"/>
       <c r="H66" s="15"/>
     </row>
-    <row r="67" spans="6:24" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="67" spans="6:33" ht="26.25" x14ac:dyDescent="0.4">
       <c r="F67" s="11"/>
       <c r="G67" s="11"/>
       <c r="H67" s="15"/>
@@ -1400,7 +1529,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="70" spans="6:24" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="70" spans="6:33" ht="31.5" x14ac:dyDescent="0.5">
       <c r="F70" s="17" t="s">
         <v>83</v>
       </c>
@@ -1409,14 +1538,188 @@
       <c r="I70" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="M70" s="8"/>
+      <c r="M70" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="X70" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="AG70" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="72" spans="6:33" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I72" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="M72" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="X72" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="74" spans="6:33" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I74" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="M74" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="X74" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="76" spans="6:33" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I76" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="M76" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="X76" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="78" spans="6:33" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I78" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="M78" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="X78" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="80" spans="6:33" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I80" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="M80" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="X80" s="8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="82" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I82" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="M82" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="X82" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="84" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I84" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="M84" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="X84" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="86" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I86" s="8">
+        <v>1517</v>
+      </c>
+      <c r="M86" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="X86" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="88" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I88" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="M88" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="X88" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="90" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I90" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="M90" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="X90" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="92" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I92" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="M92" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="X92" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="94" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I94" s="8">
+        <v>1848</v>
+      </c>
+      <c r="M94" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="X94" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="96" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I96" s="8">
+        <v>1866</v>
+      </c>
+      <c r="M96" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="X96" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="98" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I98" s="8">
+        <v>1871</v>
+      </c>
+      <c r="M98" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="X98" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="100" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I100" s="8">
+        <v>1888</v>
+      </c>
+      <c r="M100" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="X100" s="8" t="s">
+        <v>127</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="AG5" r:id="rId1" xr:uid="{49191068-0441-487B-9A7D-F06AE824FFC0}"/>
     <hyperlink ref="AG7" r:id="rId2" xr:uid="{0A5B0AB2-0153-4C97-B431-66F9538BD799}"/>
+    <hyperlink ref="AG70" r:id="rId3" xr:uid="{10FEDE2B-5CA7-4BB0-9B03-AE03E9730277}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
frontend belerakva bele is kezdtem 2023.04.20
</commit_message>
<xml_diff>
--- a/document_database/Adatgyűjtés/országok történetei.xlsx
+++ b/document_database/Adatgyűjtés/országok történetei.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20397"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47303C6-1693-4BBB-BA7F-C0ADD7096C38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0017432-F94B-464C-861C-D0D514DCBC17}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="146">
   <si>
     <t>Magyarország</t>
   </si>
@@ -404,6 +404,60 @@
   </si>
   <si>
     <t>Három császár éve.txt</t>
+  </si>
+  <si>
+    <t>Németország az első világháborúban.</t>
+  </si>
+  <si>
+    <t>Német elsővilágháború.txt</t>
+  </si>
+  <si>
+    <t>1918-1933</t>
+  </si>
+  <si>
+    <t>Weimari Köztársaság</t>
+  </si>
+  <si>
+    <t>Weimar.txt</t>
+  </si>
+  <si>
+    <t>1933-1945</t>
+  </si>
+  <si>
+    <t>Nemzetiszocializmus és 2. világháború</t>
+  </si>
+  <si>
+    <t>Nemzetiszocializmus és 2. világháború.txt</t>
+  </si>
+  <si>
+    <t>1945-1990</t>
+  </si>
+  <si>
+    <t>Kettéosztott Németország</t>
+  </si>
+  <si>
+    <t>Kettéosztott Németország.txt</t>
+  </si>
+  <si>
+    <t>NDK</t>
+  </si>
+  <si>
+    <t>NDK.txt</t>
+  </si>
+  <si>
+    <t>NSZK</t>
+  </si>
+  <si>
+    <t>NSZK.txt</t>
+  </si>
+  <si>
+    <t>Újraegyesült Németország</t>
+  </si>
+  <si>
+    <t>Újraegyesült Németország.txt</t>
+  </si>
+  <si>
+    <t>USA</t>
   </si>
 </sst>
 </file>
@@ -465,7 +519,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -520,6 +574,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -534,7 +600,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -553,6 +619,9 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hivatkozás" xfId="1" builtinId="8"/>
@@ -839,10 +908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:AI100"/>
+  <dimension ref="B3:AI117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X101" sqref="X101"/>
+    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O116" sqref="O116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1548,7 +1617,11 @@
         <v>86</v>
       </c>
     </row>
+    <row r="71" spans="6:33" x14ac:dyDescent="0.25">
+      <c r="H71" s="18"/>
+    </row>
     <row r="72" spans="6:33" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="H72" s="18"/>
       <c r="I72" s="8" t="s">
         <v>87</v>
       </c>
@@ -1559,7 +1632,11 @@
         <v>92</v>
       </c>
     </row>
+    <row r="73" spans="6:33" x14ac:dyDescent="0.25">
+      <c r="H73" s="18"/>
+    </row>
     <row r="74" spans="6:33" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="H74" s="18"/>
       <c r="I74" s="8" t="s">
         <v>90</v>
       </c>
@@ -1570,7 +1647,11 @@
         <v>93</v>
       </c>
     </row>
+    <row r="75" spans="6:33" x14ac:dyDescent="0.25">
+      <c r="H75" s="18"/>
+    </row>
     <row r="76" spans="6:33" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="H76" s="18"/>
       <c r="I76" s="8" t="s">
         <v>94</v>
       </c>
@@ -1581,7 +1662,11 @@
         <v>99</v>
       </c>
     </row>
+    <row r="77" spans="6:33" x14ac:dyDescent="0.25">
+      <c r="H77" s="18"/>
+    </row>
     <row r="78" spans="6:33" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="H78" s="18"/>
       <c r="I78" s="8" t="s">
         <v>96</v>
       </c>
@@ -1592,7 +1677,11 @@
         <v>98</v>
       </c>
     </row>
+    <row r="79" spans="6:33" x14ac:dyDescent="0.25">
+      <c r="H79" s="18"/>
+    </row>
     <row r="80" spans="6:33" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="H80" s="18"/>
       <c r="I80" s="8" t="s">
         <v>100</v>
       </c>
@@ -1603,7 +1692,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="82" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="81" spans="8:24" x14ac:dyDescent="0.25">
+      <c r="H81" s="18"/>
+    </row>
+    <row r="82" spans="8:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="H82" s="18"/>
       <c r="I82" s="8" t="s">
         <v>103</v>
       </c>
@@ -1614,7 +1707,11 @@
         <v>105</v>
       </c>
     </row>
-    <row r="84" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="83" spans="8:24" x14ac:dyDescent="0.25">
+      <c r="H83" s="18"/>
+    </row>
+    <row r="84" spans="8:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="H84" s="18"/>
       <c r="I84" s="8" t="s">
         <v>106</v>
       </c>
@@ -1625,7 +1722,11 @@
         <v>108</v>
       </c>
     </row>
-    <row r="86" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="85" spans="8:24" x14ac:dyDescent="0.25">
+      <c r="H85" s="18"/>
+    </row>
+    <row r="86" spans="8:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="H86" s="18"/>
       <c r="I86" s="8">
         <v>1517</v>
       </c>
@@ -1636,7 +1737,11 @@
         <v>110</v>
       </c>
     </row>
-    <row r="88" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="87" spans="8:24" x14ac:dyDescent="0.25">
+      <c r="H87" s="18"/>
+    </row>
+    <row r="88" spans="8:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="H88" s="18"/>
       <c r="I88" s="8" t="s">
         <v>111</v>
       </c>
@@ -1647,7 +1752,11 @@
         <v>113</v>
       </c>
     </row>
-    <row r="90" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="89" spans="8:24" x14ac:dyDescent="0.25">
+      <c r="H89" s="18"/>
+    </row>
+    <row r="90" spans="8:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="H90" s="18"/>
       <c r="I90" s="8" t="s">
         <v>114</v>
       </c>
@@ -1658,7 +1767,11 @@
         <v>116</v>
       </c>
     </row>
-    <row r="92" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="91" spans="8:24" x14ac:dyDescent="0.25">
+      <c r="H91" s="18"/>
+    </row>
+    <row r="92" spans="8:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="H92" s="18"/>
       <c r="I92" s="8" t="s">
         <v>117</v>
       </c>
@@ -1669,7 +1782,11 @@
         <v>119</v>
       </c>
     </row>
-    <row r="94" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="93" spans="8:24" x14ac:dyDescent="0.25">
+      <c r="H93" s="18"/>
+    </row>
+    <row r="94" spans="8:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="H94" s="18"/>
       <c r="I94" s="8">
         <v>1848</v>
       </c>
@@ -1680,7 +1797,11 @@
         <v>121</v>
       </c>
     </row>
-    <row r="96" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="95" spans="8:24" x14ac:dyDescent="0.25">
+      <c r="H95" s="18"/>
+    </row>
+    <row r="96" spans="8:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="H96" s="18"/>
       <c r="I96" s="8">
         <v>1866</v>
       </c>
@@ -1691,7 +1812,11 @@
         <v>123</v>
       </c>
     </row>
-    <row r="98" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="97" spans="8:24" x14ac:dyDescent="0.25">
+      <c r="H97" s="18"/>
+    </row>
+    <row r="98" spans="8:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="H98" s="18"/>
       <c r="I98" s="8">
         <v>1871</v>
       </c>
@@ -1702,7 +1827,11 @@
         <v>126</v>
       </c>
     </row>
-    <row r="100" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="99" spans="8:24" x14ac:dyDescent="0.25">
+      <c r="H99" s="18"/>
+    </row>
+    <row r="100" spans="8:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="H100" s="18"/>
       <c r="I100" s="8">
         <v>1888</v>
       </c>
@@ -1712,6 +1841,117 @@
       <c r="X100" s="8" t="s">
         <v>127</v>
       </c>
+    </row>
+    <row r="101" spans="8:24" x14ac:dyDescent="0.25">
+      <c r="H101" s="18"/>
+    </row>
+    <row r="102" spans="8:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="H102" s="18"/>
+      <c r="I102" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="M102" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="X102" s="8" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="103" spans="8:24" x14ac:dyDescent="0.25">
+      <c r="H103" s="18"/>
+    </row>
+    <row r="104" spans="8:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="H104" s="18"/>
+      <c r="I104" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="M104" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="X104" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="105" spans="8:24" x14ac:dyDescent="0.25">
+      <c r="H105" s="18"/>
+    </row>
+    <row r="106" spans="8:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="H106" s="18"/>
+      <c r="I106" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="M106" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="X106" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="107" spans="8:24" x14ac:dyDescent="0.25">
+      <c r="H107" s="18"/>
+    </row>
+    <row r="108" spans="8:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="H108" s="18"/>
+      <c r="I108" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="M108" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="X108" s="8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="109" spans="8:24" x14ac:dyDescent="0.25">
+      <c r="H109" s="18"/>
+    </row>
+    <row r="110" spans="8:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="H110" s="18"/>
+      <c r="I110" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="M110" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="X110" s="8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="111" spans="8:24" x14ac:dyDescent="0.25">
+      <c r="H111" s="18"/>
+    </row>
+    <row r="112" spans="8:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="H112" s="18"/>
+      <c r="I112" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="M112" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="X112" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="113" spans="7:24" x14ac:dyDescent="0.25">
+      <c r="H113" s="18"/>
+    </row>
+    <row r="114" spans="7:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="H114" s="18"/>
+      <c r="I114" s="8">
+        <v>1990</v>
+      </c>
+      <c r="M114" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="X114" s="8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="117" spans="7:24" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="G117" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="H117" s="20"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
frontend haladás 2023.04.21 (iskolából)
</commit_message>
<xml_diff>
--- a/document_database/Adatgyűjtés/országok történetei.xlsx
+++ b/document_database/Adatgyűjtés/országok történetei.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20397"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0017432-F94B-464C-861C-D0D514DCBC17}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC8502A-4738-4B81-A6FB-44908CF29DE9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="148">
   <si>
     <t>Magyarország</t>
   </si>
@@ -458,6 +458,12 @@
   </si>
   <si>
     <t>USA</t>
+  </si>
+  <si>
+    <t>Kolumbusz Kristóf felfedezi Amerikát</t>
+  </si>
+  <si>
+    <t>Kolombusz.txt</t>
   </si>
 </sst>
 </file>
@@ -910,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:AI117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O116" sqref="O116"/>
+    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T106" sqref="T106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1952,6 +1958,15 @@
         <v>145</v>
       </c>
       <c r="H117" s="20"/>
+      <c r="I117" s="8">
+        <v>1492</v>
+      </c>
+      <c r="M117" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="X117" s="8" t="s">
+        <v>147</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
design kész, adatgyűjtés kész
</commit_message>
<xml_diff>
--- a/document_database/Adatgyűjtés/országok történetei.xlsx
+++ b/document_database/Adatgyűjtés/országok történetei.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="301">
   <si>
     <t>Magyarország</t>
   </si>
@@ -799,6 +799,129 @@
   </si>
   <si>
     <t>Babenberg.txt</t>
+  </si>
+  <si>
+    <t>1260-1397</t>
+  </si>
+  <si>
+    <t>Inkvizíció Ausztriában</t>
+  </si>
+  <si>
+    <t>osztrák ink.txt</t>
+  </si>
+  <si>
+    <t>A nagyhatalom születése</t>
+  </si>
+  <si>
+    <t>Nagyhatalom.txt</t>
+  </si>
+  <si>
+    <t>1526-1683</t>
+  </si>
+  <si>
+    <t>Osztrák-török háborúk</t>
+  </si>
+  <si>
+    <t>Osztrák-török háború.txt</t>
+  </si>
+  <si>
+    <t>Bécs ostroma</t>
+  </si>
+  <si>
+    <t>Bécs ostroma.txt</t>
+  </si>
+  <si>
+    <t>1576-1648</t>
+  </si>
+  <si>
+    <t>Ellenreformáció és a 30 éves háború</t>
+  </si>
+  <si>
+    <t>30 éves háború.txt</t>
+  </si>
+  <si>
+    <t>Magyarországi török uralom vége</t>
+  </si>
+  <si>
+    <t>Török uralom vége.txt</t>
+  </si>
+  <si>
+    <t>1700-1714</t>
+  </si>
+  <si>
+    <t>Spanyol örökösödési háború</t>
+  </si>
+  <si>
+    <t>örökös háború.txt</t>
+  </si>
+  <si>
+    <t>1740-1780</t>
+  </si>
+  <si>
+    <t>Mária Terézia</t>
+  </si>
+  <si>
+    <t>Mária Terézia.txt</t>
+  </si>
+  <si>
+    <t>1780-1790</t>
+  </si>
+  <si>
+    <t>2. József</t>
+  </si>
+  <si>
+    <t>2. József.txt</t>
+  </si>
+  <si>
+    <t>1797-1814</t>
+  </si>
+  <si>
+    <t>Napóleoni háborúk.txt</t>
+  </si>
+  <si>
+    <t>Magyar forradalom</t>
+  </si>
+  <si>
+    <t>Magyar forradalom.txt</t>
+  </si>
+  <si>
+    <t>1867-1918</t>
+  </si>
+  <si>
+    <t>Osztrák-Magyar Monarchia</t>
+  </si>
+  <si>
+    <t>Osztrák-Magyar Monarchia.txt</t>
+  </si>
+  <si>
+    <t>Osztrák-Magyar Monarchia az első világháborúban</t>
+  </si>
+  <si>
+    <t>OMMWW1.txt</t>
+  </si>
+  <si>
+    <t>1918-1938</t>
+  </si>
+  <si>
+    <t>Az első osztrák köztársaság</t>
+  </si>
+  <si>
+    <t>Első köztársaság.txt</t>
+  </si>
+  <si>
+    <t>1938-1945</t>
+  </si>
+  <si>
+    <t>Anschluss és a második világháború</t>
+  </si>
+  <si>
+    <t>Anschluss.txt</t>
+  </si>
+  <si>
+    <t>Második osztrák köztársaság megalakulása</t>
+  </si>
+  <si>
+    <t>Második köztársaság.txt</t>
   </si>
 </sst>
 </file>
@@ -1259,10 +1382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:AI203"/>
+  <dimension ref="B3:AI235"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A194" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J212" sqref="J212"/>
+    <sheetView tabSelected="1" topLeftCell="A219" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U227" sqref="U227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2945,6 +3068,182 @@
         <v>259</v>
       </c>
     </row>
+    <row r="205" spans="6:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I205" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="M205" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="X205" s="8" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="207" spans="6:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I207" s="8">
+        <v>1437</v>
+      </c>
+      <c r="M207" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="X207" s="8" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="209" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I209" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="M209" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="X209" s="8" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="211" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I211" s="8">
+        <v>1529</v>
+      </c>
+      <c r="M211" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="X211" s="8" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="213" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I213" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="M213" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="X213" s="8" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="215" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I215" s="8">
+        <v>1683</v>
+      </c>
+      <c r="M215" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="X215" s="8" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="217" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I217" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="M217" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="X217" s="8" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="219" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I219" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="M219" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="X219" s="8" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="221" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I221" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="M221" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="X221" s="8" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="223" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I223" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="M223" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="X223" s="8" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="225" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I225" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="M225" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="X225" s="8" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="227" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I227" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="M227" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="X227" s="8" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="229" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I229" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="M229" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="X229" s="8" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="231" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I231" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="M231" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="X231" s="8" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="233" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I233" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="M233" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="X233" s="8" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="235" spans="9:24" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="I235" s="8">
+        <v>1945</v>
+      </c>
+      <c r="M235" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="X235" s="8" t="s">
+        <v>300</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="AG5" r:id="rId1"/>

</xml_diff>